<commit_message>
IntelliJ IDE - Wrapping into one test case_Review comment_1
</commit_message>
<xml_diff>
--- a/src/test/resources/ProgData.xlsx
+++ b/src/test/resources/ProgData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shanmugam Rani\eclipse-workspace\Altimetrik.MiniProjects.APIAutomation\src\test\java\DataDrivenTesting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shanmugam Rani\eclipse-workspace\Altimetrik_MiniProject_APIAutomation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF9CBE17-6029-4CDD-8216-7FDEC84643BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1CE32AB-C086-481D-B430-EF20CFA8F489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -380,7 +380,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>